<commit_message>
Added:Functionality to check the KeyWordDriven FrameWork from the facebook website
</commit_message>
<xml_diff>
--- a/src/main/java/com/bridgelabz/scenario/FBKeyWordDrivenLogin.xlsx
+++ b/src/main/java/com/bridgelabz/scenario/FBKeyWordDrivenLogin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12975" windowHeight="5025" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12975" windowHeight="5025"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="B1:G10"/>
+  <oleSize ref="A1:D15"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
   <si>
     <t>NA</t>
   </si>
@@ -76,9 +76,6 @@
     <t xml:space="preserve">id </t>
   </si>
   <si>
-    <t>pass</t>
-  </si>
-  <si>
     <t xml:space="preserve">name </t>
   </si>
   <si>
@@ -197,6 +194,12 @@
   </si>
   <si>
     <t>select and click</t>
+  </si>
+  <si>
+    <t>#pass</t>
+  </si>
+  <si>
+    <t>cssSelector</t>
   </si>
 </sst>
 </file>
@@ -553,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -619,19 +622,19 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -639,10 +642,10 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -656,10 +659,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -670,16 +673,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
       </c>
       <c r="E7" t="s">
         <v>0</v>
@@ -715,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -781,13 +784,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -798,81 +801,81 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -883,16 +886,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10">
         <v>19</v>
@@ -900,33 +903,33 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12">
         <v>1997</v>
@@ -934,30 +937,30 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>

</xml_diff>